<commit_message>
Code Checkin as part of Reset Employee Data class changes for RTI Scenarios
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition Scenario201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition Scenario201718.xlsx
@@ -4,68 +4,68 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="396" yWindow="36" windowWidth="15168" windowHeight="5400"/>
+    <workbookView windowHeight="5400" windowWidth="15168" xWindow="396" yWindow="36"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="ResetEmployeeData" sheetId="14" r:id="rId2"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM1" sheetId="6" r:id="rId3"/>
-    <sheet name="ProcessPayrollForApril" sheetId="7" r:id="rId4"/>
-    <sheet name="ProcessFinalPayrollForApril" sheetId="49" r:id="rId5"/>
-    <sheet name="TestAprilReports" sheetId="11" r:id="rId6"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM2" sheetId="15" r:id="rId7"/>
-    <sheet name="ProcessPayrollForMay" sheetId="16" r:id="rId8"/>
-    <sheet name="ProcessFinalPayrollForMay" sheetId="17" r:id="rId9"/>
-    <sheet name="TestMayReports" sheetId="18" r:id="rId10"/>
-    <sheet name="ResetNiableInCompn" sheetId="61" r:id="rId11"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM3" sheetId="51" r:id="rId12"/>
-    <sheet name="ProcessPayrollForJune" sheetId="19" r:id="rId13"/>
-    <sheet name="ProcessFinalPayrollForJune" sheetId="50" r:id="rId14"/>
-    <sheet name="TestJuneReports" sheetId="20" r:id="rId15"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM4" sheetId="21" r:id="rId16"/>
-    <sheet name="ProcessPayrollForJuly" sheetId="22" r:id="rId17"/>
-    <sheet name="ProcessFinalPayrollForJuly" sheetId="52" r:id="rId18"/>
-    <sheet name="TestJulyReports" sheetId="23" r:id="rId19"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM5" sheetId="24" r:id="rId20"/>
-    <sheet name="ProcessPayrollForAug" sheetId="25" r:id="rId21"/>
-    <sheet name="ProcessFinalPayrollForAug" sheetId="53" r:id="rId22"/>
-    <sheet name="TestAugReports" sheetId="26" r:id="rId23"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM6" sheetId="27" r:id="rId24"/>
-    <sheet name="ProcessPayrollForSep" sheetId="28" r:id="rId25"/>
-    <sheet name="ProcessFinalPayrollForSep" sheetId="54" r:id="rId26"/>
-    <sheet name="TestSepReports" sheetId="29" r:id="rId27"/>
-    <sheet name="ResetEmployeePayrollId" sheetId="62" r:id="rId28"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM7" sheetId="30" r:id="rId29"/>
-    <sheet name="ProcessPayrollForOct" sheetId="31" r:id="rId30"/>
-    <sheet name="ProcessFinalPayrollForOct" sheetId="55" r:id="rId31"/>
-    <sheet name="TestOctReports" sheetId="32" r:id="rId32"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM8" sheetId="33" r:id="rId33"/>
-    <sheet name="ProcessPayrollForNov" sheetId="34" r:id="rId34"/>
-    <sheet name="ProcessFinalPayrollForNov" sheetId="56" r:id="rId35"/>
-    <sheet name="TestNovReports" sheetId="35" r:id="rId36"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM9" sheetId="36" r:id="rId37"/>
-    <sheet name="ProcessPayrollForDec" sheetId="37" r:id="rId38"/>
-    <sheet name="ProcessFinalPayrollForDec" sheetId="57" r:id="rId39"/>
-    <sheet name="TestDecReports" sheetId="38" r:id="rId40"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM10" sheetId="39" r:id="rId41"/>
-    <sheet name="ProcessPayrollForJan" sheetId="40" r:id="rId42"/>
-    <sheet name="ProcessFinalPayrollForJan" sheetId="58" r:id="rId43"/>
-    <sheet name="TestJanReports" sheetId="41" r:id="rId44"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM11" sheetId="42" r:id="rId45"/>
-    <sheet name="ProcessPayrollForFeb" sheetId="43" r:id="rId46"/>
-    <sheet name="ProcessFinalPayrollForFeb" sheetId="59" r:id="rId47"/>
-    <sheet name="TestFebReports" sheetId="44" r:id="rId48"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM12" sheetId="45" r:id="rId49"/>
-    <sheet name="ProcessPayrollForMarch" sheetId="46" r:id="rId50"/>
-    <sheet name="ProcessFinalPayrollForMarch" sheetId="60" r:id="rId51"/>
-    <sheet name="TestMarchReports" sheetId="47" r:id="rId52"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="ResetEmployeeData" r:id="rId2" sheetId="14"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM1" r:id="rId3" sheetId="6"/>
+    <sheet name="ProcessPayrollForApril" r:id="rId4" sheetId="7"/>
+    <sheet name="ProcessFinalPayrollForApril" r:id="rId5" sheetId="49"/>
+    <sheet name="TestAprilReports" r:id="rId6" sheetId="11"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM2" r:id="rId7" sheetId="15"/>
+    <sheet name="ProcessPayrollForMay" r:id="rId8" sheetId="16"/>
+    <sheet name="ProcessFinalPayrollForMay" r:id="rId9" sheetId="17"/>
+    <sheet name="TestMayReports" r:id="rId10" sheetId="18"/>
+    <sheet name="ResetNiableInCompn" r:id="rId11" sheetId="61"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM3" r:id="rId12" sheetId="51"/>
+    <sheet name="ProcessPayrollForJune" r:id="rId13" sheetId="19"/>
+    <sheet name="ProcessFinalPayrollForJune" r:id="rId14" sheetId="50"/>
+    <sheet name="TestJuneReports" r:id="rId15" sheetId="20"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM4" r:id="rId16" sheetId="21"/>
+    <sheet name="ProcessPayrollForJuly" r:id="rId17" sheetId="22"/>
+    <sheet name="ProcessFinalPayrollForJuly" r:id="rId18" sheetId="52"/>
+    <sheet name="TestJulyReports" r:id="rId19" sheetId="23"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM5" r:id="rId20" sheetId="24"/>
+    <sheet name="ProcessPayrollForAug" r:id="rId21" sheetId="25"/>
+    <sheet name="ProcessFinalPayrollForAug" r:id="rId22" sheetId="53"/>
+    <sheet name="TestAugReports" r:id="rId23" sheetId="26"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM6" r:id="rId24" sheetId="27"/>
+    <sheet name="ProcessPayrollForSep" r:id="rId25" sheetId="28"/>
+    <sheet name="ProcessFinalPayrollForSep" r:id="rId26" sheetId="54"/>
+    <sheet name="TestSepReports" r:id="rId27" sheetId="29"/>
+    <sheet name="ResetEmployeePayrollId" r:id="rId28" sheetId="62"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM7" r:id="rId29" sheetId="30"/>
+    <sheet name="ProcessPayrollForOct" r:id="rId30" sheetId="31"/>
+    <sheet name="ProcessFinalPayrollForOct" r:id="rId31" sheetId="55"/>
+    <sheet name="TestOctReports" r:id="rId32" sheetId="32"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM8" r:id="rId33" sheetId="33"/>
+    <sheet name="ProcessPayrollForNov" r:id="rId34" sheetId="34"/>
+    <sheet name="ProcessFinalPayrollForNov" r:id="rId35" sheetId="56"/>
+    <sheet name="TestNovReports" r:id="rId36" sheetId="35"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM9" r:id="rId37" sheetId="36"/>
+    <sheet name="ProcessPayrollForDec" r:id="rId38" sheetId="37"/>
+    <sheet name="ProcessFinalPayrollForDec" r:id="rId39" sheetId="57"/>
+    <sheet name="TestDecReports" r:id="rId40" sheetId="38"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM10" r:id="rId41" sheetId="39"/>
+    <sheet name="ProcessPayrollForJan" r:id="rId42" sheetId="40"/>
+    <sheet name="ProcessFinalPayrollForJan" r:id="rId43" sheetId="58"/>
+    <sheet name="TestJanReports" r:id="rId44" sheetId="41"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM11" r:id="rId45" sheetId="42"/>
+    <sheet name="ProcessPayrollForFeb" r:id="rId46" sheetId="43"/>
+    <sheet name="ProcessFinalPayrollForFeb" r:id="rId47" sheetId="59"/>
+    <sheet name="TestFebReports" r:id="rId48" sheetId="44"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM12" r:id="rId49" sheetId="45"/>
+    <sheet name="ProcessPayrollForMarch" r:id="rId50" sheetId="46"/>
+    <sheet name="ProcessFinalPayrollForMarch" r:id="rId51" sheetId="60"/>
+    <sheet name="TestMarchReports" r:id="rId52" sheetId="47"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="171">
   <si>
     <t>TC</t>
   </si>
@@ -584,6 +584,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -637,74 +638,74 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2"/>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -721,10 +722,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -882,7 +883,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -891,13 +892,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -907,7 +908,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -916,7 +917,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -925,7 +926,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -935,12 +936,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -971,7 +972,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -990,7 +991,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1002,7 +1003,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1011,13 +1012,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1031,7 +1032,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1045,7 +1046,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>153</v>
       </c>
@@ -1059,7 +1060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -1073,7 +1074,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1087,7 +1088,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -1101,7 +1102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -1115,7 +1116,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1129,7 +1130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1143,7 +1144,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>97</v>
       </c>
@@ -1157,7 +1158,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1171,7 +1172,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>159</v>
       </c>
@@ -1185,7 +1186,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1199,7 +1200,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -1213,7 +1214,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>100</v>
       </c>
@@ -1227,7 +1228,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1760,12 +1761,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -1774,22 +1775,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="36.44140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="27" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="21.6640625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="36.44140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="25.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="21.6640625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="20.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -1842,7 +1843,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="62.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="62.4" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>91</v>
       </c>
@@ -1891,15 +1892,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1908,14 +1909,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="9.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1938,7 +1939,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>92</v>
       </c>
@@ -1958,12 +1959,12 @@
       <c r="G2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1972,15 +1973,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -2009,7 +2010,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>92</v>
       </c>
@@ -2033,12 +2034,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -2047,22 +2048,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="40.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.88671875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="31.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -2106,7 +2107,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>91</v>
       </c>
@@ -2146,14 +2147,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -2162,16 +2163,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="36.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="24.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="36.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -2215,7 +2216,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>91</v>
       </c>
@@ -2255,14 +2256,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -2271,23 +2272,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.44140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="22.6640625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="6.5546875" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="6.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="6.5546875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="6.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -2340,7 +2341,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>91</v>
       </c>
@@ -2389,14 +2390,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2405,15 +2406,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -2442,7 +2443,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="48" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>92</v>
       </c>
@@ -2466,12 +2467,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -2480,21 +2481,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.88671875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="41.5546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.33203125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="41.5546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -2538,7 +2539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>91</v>
       </c>
@@ -2577,12 +2578,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -2591,18 +2592,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="34.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.33203125" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="25.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -2646,7 +2647,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>91</v>
       </c>
@@ -2686,14 +2687,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -2702,23 +2703,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="40.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="21.6640625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.88671875" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="5.88671875" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="5.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="21.6640625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="9.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="5.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="5.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -2771,7 +2772,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>91</v>
       </c>
@@ -2819,12 +2820,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2833,13 +2834,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="8.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="8.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -2862,7 +2863,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>92</v>
       </c>
@@ -2882,13 +2883,13 @@
       <c r="G2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2897,16 +2898,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -2935,7 +2936,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="48" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>92</v>
       </c>
@@ -2959,12 +2960,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -2973,21 +2974,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="32.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -3031,7 +3032,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>91</v>
       </c>
@@ -3070,12 +3071,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -3084,14 +3085,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="38.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="22.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="38.88671875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="22.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -3135,7 +3136,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>91</v>
       </c>
@@ -3175,14 +3176,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -3191,23 +3192,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="39.44140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="22.33203125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.44140625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="6.33203125" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="6.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="39.44140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="9.44140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="6.33203125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="6.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -3260,7 +3261,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>91</v>
       </c>
@@ -3308,12 +3309,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3322,15 +3323,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="48.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -3359,7 +3360,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="34.200000000000003" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>92</v>
       </c>
@@ -3383,12 +3384,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -3397,23 +3398,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="43.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.33203125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.6640625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="43.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="43.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.6640625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.5546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -3457,7 +3458,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="65.400000000000006" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>91</v>
       </c>
@@ -3496,12 +3497,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3510,13 +3511,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="44.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="25.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -3560,7 +3561,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>91</v>
       </c>
@@ -3600,14 +3601,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -3616,20 +3617,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.88671875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="38.6640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="21.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="38.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="21.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -3682,7 +3683,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>91</v>
       </c>
@@ -3730,12 +3731,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3744,11 +3745,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -3765,7 +3766,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>92</v>
       </c>
@@ -3779,13 +3780,13 @@
       <c r="E2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3794,15 +3795,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -3831,7 +3832,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="45.6" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>92</v>
       </c>
@@ -3855,12 +3856,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3869,13 +3870,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -3904,7 +3905,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>92</v>
       </c>
@@ -3928,13 +3929,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -3943,23 +3944,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.33203125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.33203125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.33203125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.33203125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.33203125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -4003,7 +4004,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>91</v>
       </c>
@@ -4042,12 +4043,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -4056,13 +4057,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="34.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -4106,7 +4107,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>91</v>
       </c>
@@ -4146,14 +4147,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -4162,21 +4163,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="23.6640625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.88671875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.5546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -4229,7 +4230,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>91</v>
       </c>
@@ -4277,12 +4278,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4291,15 +4292,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="51.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="51.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -4328,7 +4329,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="37.200000000000003" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>92</v>
       </c>
@@ -4352,12 +4353,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -4366,21 +4367,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48.109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="31.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -4424,7 +4425,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>91</v>
       </c>
@@ -4463,12 +4464,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -4477,13 +4478,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="53.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="42.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -4527,7 +4528,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>91</v>
       </c>
@@ -4567,14 +4568,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -4583,21 +4584,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.88671875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="22" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="11.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -4650,7 +4651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>91</v>
       </c>
@@ -4698,12 +4699,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -4712,16 +4713,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="48.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -4750,7 +4751,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="40.950000000000003" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>92</v>
       </c>
@@ -4774,12 +4775,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -4788,21 +4789,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="39.5546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.44140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="39.5546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.44140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -4846,7 +4847,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>91</v>
       </c>
@@ -4885,12 +4886,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -4899,16 +4900,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="35.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="35.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -4952,7 +4953,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>91</v>
       </c>
@@ -4992,14 +4993,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -5008,21 +5009,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.5546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.5546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.5546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -5066,7 +5067,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>91</v>
       </c>
@@ -5106,15 +5107,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -5123,21 +5124,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="36.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.88671875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="24" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="36.88671875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.5546875" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="12.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -5190,7 +5191,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>91</v>
       </c>
@@ -5238,12 +5239,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5252,15 +5253,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="47.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="47.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -5289,7 +5290,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="40.200000000000003" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>92</v>
       </c>
@@ -5313,12 +5314,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -5327,21 +5328,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.44140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.44140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -5385,7 +5386,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>91</v>
       </c>
@@ -5424,12 +5425,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -5438,13 +5439,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -5488,7 +5489,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>91</v>
       </c>
@@ -5528,14 +5529,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -5544,21 +5545,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="24.33203125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.33203125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="12.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -5611,7 +5612,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>91</v>
       </c>
@@ -5659,12 +5660,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5673,15 +5674,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="47.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="47.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -5710,7 +5711,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="39" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>92</v>
       </c>
@@ -5734,12 +5735,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -5748,21 +5749,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.88671875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="40.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.88671875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -5806,7 +5807,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>91</v>
       </c>
@@ -5845,12 +5846,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -5859,17 +5860,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -5913,7 +5914,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>91</v>
       </c>
@@ -5953,14 +5954,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -5969,20 +5970,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="40.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="24.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="32.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.88671875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -6035,7 +6036,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>91</v>
       </c>
@@ -6083,12 +6084,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6097,16 +6098,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="10.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -6135,7 +6136,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="40.950000000000003" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>92</v>
       </c>
@@ -6159,12 +6160,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -6173,21 +6174,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="41.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.33203125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="41.88671875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -6231,7 +6232,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>91</v>
       </c>
@@ -6271,14 +6272,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -6287,20 +6288,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="33.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.33203125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.44140625" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="33.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.5546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.44140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -6344,7 +6345,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>91</v>
       </c>
@@ -6384,14 +6385,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK" r:id="rId1" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -6400,21 +6401,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="43.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.33203125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="43.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.5546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -6458,7 +6459,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>91</v>
       </c>
@@ -6498,15 +6499,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
-    <hyperlink ref="E2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK" r:id="rId2" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -6515,20 +6516,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.6640625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="26.109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="21.88671875" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="16.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="47.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="20.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.6640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="26.109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="21.88671875" collapsed="true"/>
+    <col min="13" max="14" customWidth="true" width="16.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -6581,7 +6582,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>91</v>
       </c>
@@ -6630,15 +6631,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK" r:id="rId1" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -6647,23 +6648,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="43.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.33203125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="35.88671875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="33.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="31.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="43.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="35.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="33.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="1" s="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>18</v>
       </c>
@@ -6716,7 +6717,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="62.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="62.4" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>91</v>
       </c>
@@ -6765,15 +6766,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6782,14 +6783,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="47.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -6818,7 +6819,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>92</v>
       </c>
@@ -6842,12 +6843,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -6856,21 +6857,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -6914,7 +6915,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="62.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="62.4" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>91</v>
       </c>
@@ -6954,14 +6955,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -6970,21 +6971,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="36.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.88671875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="40.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="36.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.88671875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -7028,7 +7029,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>91</v>
       </c>
@@ -7068,8 +7069,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Month8 and RTI 1st scenario Annual salary commiting
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition Scenario201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition Scenario201718.xlsx
@@ -1,76 +1,76 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="30" windowWidth="15165" windowHeight="5400" activeTab="3"/>
+    <workbookView activeTab="3" windowHeight="5400" windowWidth="15165" xWindow="390" yWindow="30"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="ResetEmployeeData" sheetId="14" r:id="rId2"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM1" sheetId="6" r:id="rId3"/>
-    <sheet name="ProcessPayrollForApril" sheetId="7" r:id="rId4"/>
-    <sheet name="ProcessFinalPayrollForApril" sheetId="49" r:id="rId5"/>
-    <sheet name="TestAprilReports" sheetId="11" r:id="rId6"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM2" sheetId="15" r:id="rId7"/>
-    <sheet name="ProcessPayrollForMay" sheetId="16" r:id="rId8"/>
-    <sheet name="ProcessFinalPayrollForMay" sheetId="17" r:id="rId9"/>
-    <sheet name="TestMayReports" sheetId="18" r:id="rId10"/>
-    <sheet name="ResetNiableInCompn" sheetId="61" r:id="rId11"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM3" sheetId="51" r:id="rId12"/>
-    <sheet name="ProcessPayrollForJune" sheetId="19" r:id="rId13"/>
-    <sheet name="ProcessFinalPayrollForJune" sheetId="50" r:id="rId14"/>
-    <sheet name="TestJuneReports" sheetId="20" r:id="rId15"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM4" sheetId="21" r:id="rId16"/>
-    <sheet name="ProcessPayrollForJuly" sheetId="22" r:id="rId17"/>
-    <sheet name="ProcessFinalPayrollForJuly" sheetId="52" r:id="rId18"/>
-    <sheet name="TestJulyReports" sheetId="23" r:id="rId19"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM5" sheetId="24" r:id="rId20"/>
-    <sheet name="ProcessPayrollForAug" sheetId="25" r:id="rId21"/>
-    <sheet name="ProcessFinalPayrollForAug" sheetId="53" r:id="rId22"/>
-    <sheet name="TestAugReports" sheetId="26" r:id="rId23"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM6" sheetId="27" r:id="rId24"/>
-    <sheet name="ProcessPayrollForSep" sheetId="28" r:id="rId25"/>
-    <sheet name="ProcessFinalPayrollForSep" sheetId="54" r:id="rId26"/>
-    <sheet name="TestSepReports" sheetId="29" r:id="rId27"/>
-    <sheet name="ResetEmployeePayrollId" sheetId="62" r:id="rId28"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM7" sheetId="30" r:id="rId29"/>
-    <sheet name="ProcessPayrollForOct" sheetId="31" r:id="rId30"/>
-    <sheet name="ProcessFinalPayrollForOct" sheetId="55" r:id="rId31"/>
-    <sheet name="TestOctReports" sheetId="32" r:id="rId32"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM8" sheetId="33" r:id="rId33"/>
-    <sheet name="ProcessPayrollForNov" sheetId="34" r:id="rId34"/>
-    <sheet name="ProcessFinalPayrollForNov" sheetId="56" r:id="rId35"/>
-    <sheet name="TestNovReports" sheetId="35" r:id="rId36"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM9" sheetId="36" r:id="rId37"/>
-    <sheet name="ProcessPayrollForDec" sheetId="37" r:id="rId38"/>
-    <sheet name="ProcessFinalPayrollForDec" sheetId="57" r:id="rId39"/>
-    <sheet name="TestDecReports" sheetId="38" r:id="rId40"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM10" sheetId="39" r:id="rId41"/>
-    <sheet name="ProcessPayrollForJan" sheetId="40" r:id="rId42"/>
-    <sheet name="ProcessFinalPayrollForJan" sheetId="58" r:id="rId43"/>
-    <sheet name="TestJanReports" sheetId="41" r:id="rId44"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM11" sheetId="42" r:id="rId45"/>
-    <sheet name="ProcessPayrollForFeb" sheetId="43" r:id="rId46"/>
-    <sheet name="ProcessFinalPayrollForFeb" sheetId="59" r:id="rId47"/>
-    <sheet name="TestFebReports" sheetId="44" r:id="rId48"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM12" sheetId="45" r:id="rId49"/>
-    <sheet name="ProcessPayrollForMarch" sheetId="46" r:id="rId50"/>
-    <sheet name="ProcessFinalPayrollForMarch" sheetId="60" r:id="rId51"/>
-    <sheet name="TestMarchReports" sheetId="47" r:id="rId52"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="ResetEmployeeData" r:id="rId2" sheetId="14"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM1" r:id="rId3" sheetId="6"/>
+    <sheet name="ProcessPayrollForApril" r:id="rId4" sheetId="7"/>
+    <sheet name="ProcessFinalPayrollForApril" r:id="rId5" sheetId="49"/>
+    <sheet name="TestAprilReports" r:id="rId6" sheetId="11"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM2" r:id="rId7" sheetId="15"/>
+    <sheet name="ProcessPayrollForMay" r:id="rId8" sheetId="16"/>
+    <sheet name="ProcessFinalPayrollForMay" r:id="rId9" sheetId="17"/>
+    <sheet name="TestMayReports" r:id="rId10" sheetId="18"/>
+    <sheet name="ResetNiableInCompn" r:id="rId11" sheetId="61"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM3" r:id="rId12" sheetId="51"/>
+    <sheet name="ProcessPayrollForJune" r:id="rId13" sheetId="19"/>
+    <sheet name="ProcessFinalPayrollForJune" r:id="rId14" sheetId="50"/>
+    <sheet name="TestJuneReports" r:id="rId15" sheetId="20"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM4" r:id="rId16" sheetId="21"/>
+    <sheet name="ProcessPayrollForJuly" r:id="rId17" sheetId="22"/>
+    <sheet name="ProcessFinalPayrollForJuly" r:id="rId18" sheetId="52"/>
+    <sheet name="TestJulyReports" r:id="rId19" sheetId="23"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM5" r:id="rId20" sheetId="24"/>
+    <sheet name="ProcessPayrollForAug" r:id="rId21" sheetId="25"/>
+    <sheet name="ProcessFinalPayrollForAug" r:id="rId22" sheetId="53"/>
+    <sheet name="TestAugReports" r:id="rId23" sheetId="26"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM6" r:id="rId24" sheetId="27"/>
+    <sheet name="ProcessPayrollForSep" r:id="rId25" sheetId="28"/>
+    <sheet name="ProcessFinalPayrollForSep" r:id="rId26" sheetId="54"/>
+    <sheet name="TestSepReports" r:id="rId27" sheetId="29"/>
+    <sheet name="ResetEmployeePayrollId" r:id="rId28" sheetId="62"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM7" r:id="rId29" sheetId="30"/>
+    <sheet name="ProcessPayrollForOct" r:id="rId30" sheetId="31"/>
+    <sheet name="ProcessFinalPayrollForOct" r:id="rId31" sheetId="55"/>
+    <sheet name="TestOctReports" r:id="rId32" sheetId="32"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM8" r:id="rId33" sheetId="33"/>
+    <sheet name="ProcessPayrollForNov" r:id="rId34" sheetId="34"/>
+    <sheet name="ProcessFinalPayrollForNov" r:id="rId35" sheetId="56"/>
+    <sheet name="TestNovReports" r:id="rId36" sheetId="35"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM9" r:id="rId37" sheetId="36"/>
+    <sheet name="ProcessPayrollForDec" r:id="rId38" sheetId="37"/>
+    <sheet name="ProcessFinalPayrollForDec" r:id="rId39" sheetId="57"/>
+    <sheet name="TestDecReports" r:id="rId40" sheetId="38"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM10" r:id="rId41" sheetId="39"/>
+    <sheet name="ProcessPayrollForJan" r:id="rId42" sheetId="40"/>
+    <sheet name="ProcessFinalPayrollForJan" r:id="rId43" sheetId="58"/>
+    <sheet name="TestJanReports" r:id="rId44" sheetId="41"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM11" r:id="rId45" sheetId="42"/>
+    <sheet name="ProcessPayrollForFeb" r:id="rId46" sheetId="43"/>
+    <sheet name="ProcessFinalPayrollForFeb" r:id="rId47" sheetId="59"/>
+    <sheet name="TestFebReports" r:id="rId48" sheetId="44"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM12" r:id="rId49" sheetId="45"/>
+    <sheet name="ProcessPayrollForMarch" r:id="rId50" sheetId="46"/>
+    <sheet name="ProcessFinalPayrollForMarch" r:id="rId51" sheetId="60"/>
+    <sheet name="TestMarchReports" r:id="rId52" sheetId="47"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="171">
   <si>
     <t>TC</t>
   </si>
@@ -589,6 +589,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -642,75 +643,75 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2"/>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -727,10 +728,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -765,7 +766,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -817,7 +818,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -922,7 +923,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -931,13 +932,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -947,7 +948,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -956,7 +957,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -965,7 +966,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -975,12 +976,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1011,7 +1012,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1030,7 +1031,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1042,7 +1043,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1051,10 +1052,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1800,12 +1801,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1814,22 +1815,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="36.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.7109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="27" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="36.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="20.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -1882,7 +1883,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="62.45" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>170</v>
       </c>
@@ -1930,13 +1931,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1945,11 +1946,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1975,7 +1976,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>91</v>
       </c>
@@ -1995,12 +1996,12 @@
       <c r="G2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2009,12 +2010,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2046,7 +2047,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>91</v>
       </c>
@@ -2070,12 +2071,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2084,19 +2085,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="40.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.85546875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2143,7 +2144,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>170</v>
       </c>
@@ -2182,12 +2183,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2196,13 +2197,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="36.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="36.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2249,7 +2250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>170</v>
       </c>
@@ -2288,12 +2289,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2302,23 +2303,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="22.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="6.5703125" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="6.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="6.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -2371,7 +2372,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>170</v>
       </c>
@@ -2419,12 +2420,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2433,12 +2434,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2470,7 +2471,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="48" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>91</v>
       </c>
@@ -2494,12 +2495,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2508,18 +2509,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="41.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="41.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2566,7 +2567,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -2606,14 +2607,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2622,15 +2623,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="34.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="25.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2677,7 +2678,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -2717,14 +2718,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2733,23 +2734,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="40.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.85546875" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="5.85546875" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="5.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="5.85546875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="5.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -2802,7 +2803,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -2851,14 +2852,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2867,10 +2868,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2896,7 +2897,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>91</v>
       </c>
@@ -2916,13 +2917,13 @@
       <c r="G2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2931,13 +2932,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2969,7 +2970,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="48" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>91</v>
       </c>
@@ -2993,12 +2994,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3007,18 +3008,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.7109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3065,7 +3066,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -3105,14 +3106,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3121,11 +3122,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="38.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="22.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="38.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="22.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3172,7 +3173,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -3212,14 +3213,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3228,23 +3229,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="39.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.42578125" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="6.28515625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="6.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="39.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="6.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -3297,7 +3298,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -3346,14 +3347,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3362,12 +3363,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="48.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3399,7 +3400,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="34.15" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>91</v>
       </c>
@@ -3423,12 +3424,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3437,20 +3438,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="43.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="43.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="43.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3497,7 +3498,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="65.45" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -3537,14 +3538,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3553,10 +3554,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="44.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="25.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3603,7 +3604,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -3643,14 +3644,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3659,20 +3660,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="38.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="38.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="21.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -3725,7 +3726,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -3774,14 +3775,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3790,8 +3791,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3811,7 +3812,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>91</v>
       </c>
@@ -3825,13 +3826,13 @@
       <c r="E2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3840,12 +3841,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3877,7 +3878,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="45.6" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>91</v>
       </c>
@@ -3901,12 +3902,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3915,10 +3916,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3950,7 +3951,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>91</v>
       </c>
@@ -3974,13 +3975,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3989,20 +3990,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.28515625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4049,7 +4050,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -4089,14 +4090,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4105,10 +4106,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="34.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4155,7 +4156,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -4195,14 +4196,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4211,21 +4212,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="23.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -4278,7 +4279,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -4327,14 +4328,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4343,12 +4344,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="51.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="51.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -4380,7 +4381,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="37.15" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>91</v>
       </c>
@@ -4404,12 +4405,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4418,18 +4419,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.7109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4476,7 +4477,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -4516,14 +4517,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4532,10 +4533,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="53.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4582,7 +4583,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -4622,14 +4623,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4638,21 +4639,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="22" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="11.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -4705,7 +4706,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -4754,14 +4755,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4770,13 +4771,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="48.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -4808,7 +4809,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="40.9" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>91</v>
       </c>
@@ -4832,12 +4833,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4846,18 +4847,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="39.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="39.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4904,7 +4905,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -4944,14 +4945,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4960,13 +4961,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="35.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="35.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5013,7 +5014,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -5053,14 +5054,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -5069,18 +5070,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5703125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5127,7 +5128,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -5167,15 +5168,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5184,21 +5185,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="36.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="24" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="36.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -5251,7 +5252,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -5300,14 +5301,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5316,12 +5317,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="47.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="47.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -5353,7 +5354,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="40.15" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>91</v>
       </c>
@@ -5377,12 +5378,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5391,18 +5392,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5449,7 +5450,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -5489,14 +5490,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5505,10 +5506,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5555,7 +5556,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -5595,14 +5596,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5611,21 +5612,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -5678,7 +5679,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -5727,14 +5728,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5743,12 +5744,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="47.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="47.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -5780,7 +5781,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="39" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>91</v>
       </c>
@@ -5804,12 +5805,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5818,18 +5819,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="40.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5876,7 +5877,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -5916,14 +5917,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5932,14 +5933,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5986,7 +5987,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -6026,14 +6027,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6042,20 +6043,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="40.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="32.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -6108,7 +6109,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -6157,14 +6158,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6173,13 +6174,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6211,7 +6212,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="40.9" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>91</v>
       </c>
@@ -6235,12 +6236,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6249,18 +6250,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="41.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="41.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -6307,7 +6308,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>170</v>
       </c>
@@ -6346,12 +6347,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6360,17 +6361,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="33.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -6417,7 +6418,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -6457,15 +6458,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6474,18 +6475,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="43.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="43.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -6532,7 +6533,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -6572,15 +6573,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6589,20 +6590,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="47.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="13" max="14" customWidth="true" width="16.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -6655,7 +6656,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>170</v>
       </c>
@@ -6704,16 +6705,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId3" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6722,23 +6723,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="43.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="35.85546875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="33.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="31.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="43.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="35.85546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="33.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="1" s="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>18</v>
       </c>
@@ -6791,7 +6792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="62.45" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>170</v>
       </c>
@@ -6839,13 +6840,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6854,11 +6855,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="47.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6890,7 +6891,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>91</v>
       </c>
@@ -6914,12 +6915,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6928,18 +6929,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -6986,7 +6987,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="62.45" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>170</v>
       </c>
@@ -7025,12 +7026,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -7039,18 +7040,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="36.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="40.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="36.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -7097,7 +7098,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>170</v>
       </c>
@@ -7136,6 +7137,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
RTI Scenario 1 testing
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition Scenario201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition Scenario201718.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="3" windowHeight="5400" windowWidth="15165" xWindow="390" yWindow="30"/>
+    <workbookView activeTab="14" firstSheet="12" windowHeight="5400" windowWidth="15165" xWindow="390" yWindow="30"/>
   </bookViews>
   <sheets>
     <sheet name="first" r:id="rId1" sheetId="1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="171">
   <si>
     <t>TC</t>
   </si>
@@ -1809,8 +1809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1905,7 +1905,7 @@
       <c r="G2" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="16" t="s">
         <v>168</v>
       </c>
       <c r="I2" s="13" t="s">
@@ -2297,8 +2297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2394,7 +2394,7 @@
       <c r="G2" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="16" t="s">
         <v>168</v>
       </c>
       <c r="I2" s="13" t="s">
@@ -5064,7 +5064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -6244,8 +6244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6717,8 +6717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7034,7 +7034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Pagination Logic Implementation for Monthly and Four Weekly
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition Scenario201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition Scenario201718.xlsx
@@ -1,76 +1,76 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="30" windowWidth="15165" windowHeight="5400" firstSheet="49" activeTab="50"/>
+    <workbookView activeTab="50" firstSheet="49" windowHeight="5400" windowWidth="15165" xWindow="390" yWindow="30"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="ResetEmployeeData" sheetId="14" r:id="rId2"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM1" sheetId="6" r:id="rId3"/>
-    <sheet name="ProcessPayrollForApril" sheetId="7" r:id="rId4"/>
-    <sheet name="ProcessFinalPayrollForApril" sheetId="49" r:id="rId5"/>
-    <sheet name="TestAprilReports" sheetId="11" r:id="rId6"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM2" sheetId="15" r:id="rId7"/>
-    <sheet name="ProcessPayrollForMay" sheetId="16" r:id="rId8"/>
-    <sheet name="ProcessFinalPayrollForMay" sheetId="17" r:id="rId9"/>
-    <sheet name="TestMayReports" sheetId="18" r:id="rId10"/>
-    <sheet name="ResetNiableInCompn" sheetId="61" r:id="rId11"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM3" sheetId="51" r:id="rId12"/>
-    <sheet name="ProcessPayrollForJune" sheetId="19" r:id="rId13"/>
-    <sheet name="ProcessFinalPayrollForJune" sheetId="50" r:id="rId14"/>
-    <sheet name="TestJuneReports" sheetId="20" r:id="rId15"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM4" sheetId="21" r:id="rId16"/>
-    <sheet name="ProcessPayrollForJuly" sheetId="22" r:id="rId17"/>
-    <sheet name="ProcessFinalPayrollForJuly" sheetId="52" r:id="rId18"/>
-    <sheet name="TestJulyReports" sheetId="23" r:id="rId19"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM5" sheetId="24" r:id="rId20"/>
-    <sheet name="ProcessPayrollForAug" sheetId="25" r:id="rId21"/>
-    <sheet name="ProcessFinalPayrollForAug" sheetId="53" r:id="rId22"/>
-    <sheet name="TestAugReports" sheetId="26" r:id="rId23"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM6" sheetId="27" r:id="rId24"/>
-    <sheet name="ProcessPayrollForSep" sheetId="28" r:id="rId25"/>
-    <sheet name="ProcessFinalPayrollForSep" sheetId="54" r:id="rId26"/>
-    <sheet name="TestSepReports" sheetId="29" r:id="rId27"/>
-    <sheet name="ResetEmployeePayrollId" sheetId="62" r:id="rId28"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM7" sheetId="30" r:id="rId29"/>
-    <sheet name="ProcessPayrollForOct" sheetId="31" r:id="rId30"/>
-    <sheet name="ProcessFinalPayrollForOct" sheetId="55" r:id="rId31"/>
-    <sheet name="TestOctReports" sheetId="32" r:id="rId32"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM8" sheetId="33" r:id="rId33"/>
-    <sheet name="ProcessPayrollForNov" sheetId="34" r:id="rId34"/>
-    <sheet name="ProcessFinalPayrollForNov" sheetId="56" r:id="rId35"/>
-    <sheet name="TestNovReports" sheetId="35" r:id="rId36"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM9" sheetId="36" r:id="rId37"/>
-    <sheet name="ProcessPayrollForDec" sheetId="37" r:id="rId38"/>
-    <sheet name="ProcessFinalPayrollForDec" sheetId="57" r:id="rId39"/>
-    <sheet name="TestDecReports" sheetId="38" r:id="rId40"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM10" sheetId="39" r:id="rId41"/>
-    <sheet name="ProcessPayrollForJan" sheetId="40" r:id="rId42"/>
-    <sheet name="ProcessFinalPayrollForJan" sheetId="58" r:id="rId43"/>
-    <sheet name="TestJanReports" sheetId="41" r:id="rId44"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM11" sheetId="42" r:id="rId45"/>
-    <sheet name="ProcessPayrollForFeb" sheetId="43" r:id="rId46"/>
-    <sheet name="ProcessFinalPayrollForFeb" sheetId="59" r:id="rId47"/>
-    <sheet name="TestFebReports" sheetId="44" r:id="rId48"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM12" sheetId="45" r:id="rId49"/>
-    <sheet name="ProcessPayrollForMarch" sheetId="46" r:id="rId50"/>
-    <sheet name="ProcessFinalPayrollForMarch" sheetId="60" r:id="rId51"/>
-    <sheet name="TestMarchReports" sheetId="47" r:id="rId52"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="ResetEmployeeData" r:id="rId2" sheetId="14"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM1" r:id="rId3" sheetId="6"/>
+    <sheet name="ProcessPayrollForApril" r:id="rId4" sheetId="7"/>
+    <sheet name="ProcessFinalPayrollForApril" r:id="rId5" sheetId="49"/>
+    <sheet name="TestAprilReports" r:id="rId6" sheetId="11"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM2" r:id="rId7" sheetId="15"/>
+    <sheet name="ProcessPayrollForMay" r:id="rId8" sheetId="16"/>
+    <sheet name="ProcessFinalPayrollForMay" r:id="rId9" sheetId="17"/>
+    <sheet name="TestMayReports" r:id="rId10" sheetId="18"/>
+    <sheet name="ResetNiableInCompn" r:id="rId11" sheetId="61"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM3" r:id="rId12" sheetId="51"/>
+    <sheet name="ProcessPayrollForJune" r:id="rId13" sheetId="19"/>
+    <sheet name="ProcessFinalPayrollForJune" r:id="rId14" sheetId="50"/>
+    <sheet name="TestJuneReports" r:id="rId15" sheetId="20"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM4" r:id="rId16" sheetId="21"/>
+    <sheet name="ProcessPayrollForJuly" r:id="rId17" sheetId="22"/>
+    <sheet name="ProcessFinalPayrollForJuly" r:id="rId18" sheetId="52"/>
+    <sheet name="TestJulyReports" r:id="rId19" sheetId="23"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM5" r:id="rId20" sheetId="24"/>
+    <sheet name="ProcessPayrollForAug" r:id="rId21" sheetId="25"/>
+    <sheet name="ProcessFinalPayrollForAug" r:id="rId22" sheetId="53"/>
+    <sheet name="TestAugReports" r:id="rId23" sheetId="26"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM6" r:id="rId24" sheetId="27"/>
+    <sheet name="ProcessPayrollForSep" r:id="rId25" sheetId="28"/>
+    <sheet name="ProcessFinalPayrollForSep" r:id="rId26" sheetId="54"/>
+    <sheet name="TestSepReports" r:id="rId27" sheetId="29"/>
+    <sheet name="ResetEmployeePayrollId" r:id="rId28" sheetId="62"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM7" r:id="rId29" sheetId="30"/>
+    <sheet name="ProcessPayrollForOct" r:id="rId30" sheetId="31"/>
+    <sheet name="ProcessFinalPayrollForOct" r:id="rId31" sheetId="55"/>
+    <sheet name="TestOctReports" r:id="rId32" sheetId="32"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM8" r:id="rId33" sheetId="33"/>
+    <sheet name="ProcessPayrollForNov" r:id="rId34" sheetId="34"/>
+    <sheet name="ProcessFinalPayrollForNov" r:id="rId35" sheetId="56"/>
+    <sheet name="TestNovReports" r:id="rId36" sheetId="35"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM9" r:id="rId37" sheetId="36"/>
+    <sheet name="ProcessPayrollForDec" r:id="rId38" sheetId="37"/>
+    <sheet name="ProcessFinalPayrollForDec" r:id="rId39" sheetId="57"/>
+    <sheet name="TestDecReports" r:id="rId40" sheetId="38"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM10" r:id="rId41" sheetId="39"/>
+    <sheet name="ProcessPayrollForJan" r:id="rId42" sheetId="40"/>
+    <sheet name="ProcessFinalPayrollForJan" r:id="rId43" sheetId="58"/>
+    <sheet name="TestJanReports" r:id="rId44" sheetId="41"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM11" r:id="rId45" sheetId="42"/>
+    <sheet name="ProcessPayrollForFeb" r:id="rId46" sheetId="43"/>
+    <sheet name="ProcessFinalPayrollForFeb" r:id="rId47" sheetId="59"/>
+    <sheet name="TestFebReports" r:id="rId48" sheetId="44"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM12" r:id="rId49" sheetId="45"/>
+    <sheet name="ProcessPayrollForMarch" r:id="rId50" sheetId="46"/>
+    <sheet name="ProcessFinalPayrollForMarch" r:id="rId51" sheetId="60"/>
+    <sheet name="TestMarchReports" r:id="rId52" sheetId="47"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="176">
   <si>
     <t>TC</t>
   </si>
@@ -607,6 +607,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -666,75 +667,75 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2"/>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -751,10 +752,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -789,7 +790,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -841,7 +842,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -946,7 +947,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -955,13 +956,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -971,7 +972,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -980,7 +981,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -989,7 +990,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -999,12 +1000,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1035,7 +1036,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1054,7 +1055,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1066,7 +1067,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView topLeftCell="A67" workbookViewId="0">
@@ -1075,10 +1076,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1824,12 +1825,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1838,22 +1839,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="36.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.7109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="27" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="36.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="20.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -1906,7 +1907,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="62.45" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>171</v>
       </c>
@@ -1954,13 +1955,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1969,11 +1970,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1999,7 +2000,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>175</v>
       </c>
@@ -2019,12 +2020,12 @@
       <c r="G2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2033,12 +2034,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="72.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2070,7 +2071,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>175</v>
       </c>
@@ -2094,12 +2095,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2108,19 +2109,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="40.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.85546875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2167,7 +2168,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>170</v>
       </c>
@@ -2206,13 +2207,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2221,13 +2222,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="36.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="36.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2274,7 +2275,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>170</v>
       </c>
@@ -2313,12 +2314,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2327,23 +2328,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="22.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="6.5703125" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="6.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="6.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -2396,7 +2397,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>171</v>
       </c>
@@ -2444,12 +2445,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2458,12 +2459,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2495,7 +2496,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="48" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>175</v>
       </c>
@@ -2519,12 +2520,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2533,18 +2534,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="41.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="41.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2591,7 +2592,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>171</v>
       </c>
@@ -2630,12 +2631,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2644,15 +2645,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="34.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="25.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2699,7 +2700,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>171</v>
       </c>
@@ -2738,12 +2739,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2752,23 +2753,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="40.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.85546875" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="5.85546875" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="5.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="5.85546875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="5.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -2821,7 +2822,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>171</v>
       </c>
@@ -2869,12 +2870,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2883,10 +2884,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2912,7 +2913,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>175</v>
       </c>
@@ -2932,13 +2933,13 @@
       <c r="G2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2947,13 +2948,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2985,7 +2986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="48" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>175</v>
       </c>
@@ -3009,12 +3010,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3023,18 +3024,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.7109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3081,7 +3082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>171</v>
       </c>
@@ -3120,12 +3121,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3134,11 +3135,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="38.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="22.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="38.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="22.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3185,7 +3186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>171</v>
       </c>
@@ -3224,12 +3225,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3238,23 +3239,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="39.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.42578125" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="6.28515625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="6.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="39.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="6.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -3307,7 +3308,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>171</v>
       </c>
@@ -3355,12 +3356,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3369,12 +3370,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="48.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3406,7 +3407,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="34.15" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>175</v>
       </c>
@@ -3430,12 +3431,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3444,20 +3445,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="43.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="43.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="43.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3504,7 +3505,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="65.45" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>171</v>
       </c>
@@ -3543,12 +3544,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3557,10 +3558,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="44.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="25.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3607,7 +3608,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>171</v>
       </c>
@@ -3646,12 +3647,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3660,20 +3661,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="38.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="38.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="21.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -3726,7 +3727,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>171</v>
       </c>
@@ -3774,12 +3775,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3788,8 +3789,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3809,7 +3810,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>175</v>
       </c>
@@ -3823,13 +3824,13 @@
       <c r="E2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3838,12 +3839,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3875,7 +3876,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="45.6" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>175</v>
       </c>
@@ -3899,12 +3900,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3913,10 +3914,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3948,7 +3949,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>175</v>
       </c>
@@ -3972,13 +3973,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3987,20 +3988,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.28515625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4047,7 +4048,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>171</v>
       </c>
@@ -4086,12 +4087,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4100,10 +4101,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="34.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4150,7 +4151,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>171</v>
       </c>
@@ -4189,12 +4190,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4203,21 +4204,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="23.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -4270,7 +4271,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>171</v>
       </c>
@@ -4318,12 +4319,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4332,12 +4333,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="51.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="51.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -4369,7 +4370,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="37.15" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>175</v>
       </c>
@@ -4393,12 +4394,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4407,18 +4408,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.7109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4465,7 +4466,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>171</v>
       </c>
@@ -4504,12 +4505,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4518,10 +4519,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="53.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4568,7 +4569,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>171</v>
       </c>
@@ -4607,12 +4608,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4621,21 +4622,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="22" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="11.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -4688,7 +4689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>171</v>
       </c>
@@ -4736,12 +4737,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4750,13 +4751,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="48.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -4788,7 +4789,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="40.9" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>175</v>
       </c>
@@ -4812,12 +4813,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4826,18 +4827,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="39.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="39.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4884,7 +4885,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>173</v>
       </c>
@@ -4923,12 +4924,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4937,13 +4938,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="35.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="35.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4990,7 +4991,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>171</v>
       </c>
@@ -5029,12 +5030,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -5043,18 +5044,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5703125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5101,7 +5102,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>91</v>
       </c>
@@ -5141,15 +5142,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5158,21 +5159,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="36.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="24" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="36.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -5225,7 +5226,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>171</v>
       </c>
@@ -5273,12 +5274,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5287,12 +5288,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="47.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="47.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -5324,7 +5325,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="40.15" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>175</v>
       </c>
@@ -5348,12 +5349,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5362,18 +5363,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5420,7 +5421,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>171</v>
       </c>
@@ -5459,12 +5460,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5473,10 +5474,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5523,7 +5524,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>171</v>
       </c>
@@ -5562,12 +5563,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5576,21 +5577,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -5643,7 +5644,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>171</v>
       </c>
@@ -5691,12 +5692,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5705,12 +5706,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="47.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="47.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -5742,7 +5743,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="39" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>175</v>
       </c>
@@ -5766,12 +5767,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5780,18 +5781,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="40.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5838,7 +5839,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>171</v>
       </c>
@@ -5877,12 +5878,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5891,14 +5892,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5945,7 +5946,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>171</v>
       </c>
@@ -5984,12 +5985,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5998,20 +5999,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="40.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="32.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -6064,7 +6065,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>171</v>
       </c>
@@ -6112,12 +6113,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6126,13 +6127,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6164,7 +6165,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="40.9" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>175</v>
       </c>
@@ -6188,12 +6189,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6202,18 +6203,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="41.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="41.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -6260,7 +6261,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>170</v>
       </c>
@@ -6299,12 +6300,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6313,17 +6314,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="33.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -6370,7 +6371,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>171</v>
       </c>
@@ -6410,14 +6411,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK" r:id="rId1" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -6426,18 +6427,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="43.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="43.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -6484,7 +6485,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>171</v>
       </c>
@@ -6524,14 +6525,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK" r:id="rId1" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6540,20 +6541,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="47.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="13" max="14" customWidth="true" width="16.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -6606,7 +6607,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>171</v>
       </c>
@@ -6655,15 +6656,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000006qFmK" r:id="rId1" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6672,23 +6673,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="43.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="35.85546875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="33.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="31.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="43.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="35.85546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="33.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="1" s="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>18</v>
       </c>
@@ -6741,7 +6742,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="62.45" r="2" s="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>170</v>
       </c>
@@ -6789,13 +6790,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6804,11 +6805,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="47.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6840,7 +6841,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>175</v>
       </c>
@@ -6864,12 +6865,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6878,18 +6879,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -6936,7 +6937,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="62.45" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>171</v>
       </c>
@@ -6975,12 +6976,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6989,18 +6990,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="36.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="40.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="36.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -7047,7 +7048,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>171</v>
       </c>
@@ -7086,6 +7087,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>